<commit_message>
updated properly. Maven commands running fine
</commit_message>
<xml_diff>
--- a/src/test/resources/Test.xlsx
+++ b/src/test/resources/Test.xlsx
@@ -3,21 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium With Java\Marsh framework\newtours.demoaut.com\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC06D684-53D1-475C-B3BC-3B933070712A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{65CA8B9A-0091-4D86-B80D-07C0502B7D40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20550" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>TestName</t>
   </si>
@@ -80,16 +76,7 @@
     <t>TestData14</t>
   </si>
   <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>Flights</t>
-  </si>
-  <si>
-    <t>Hotels</t>
-  </si>
-  <si>
-    <t>Car Rentals</t>
+    <t>12/25/2019 - 12/25/2019</t>
   </si>
 </sst>
 </file>
@@ -417,7 +404,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,15 +480,9 @@
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>

</xml_diff>